<commit_message>
Update results / test
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_3.xlsx
+++ b/tests/integration_test_files/full_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6296F7D-A9C7-6A4F-BE3D-EF2324E149AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A95B481-47B6-444C-8C13-CF229398FF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40760" yWindow="500" windowWidth="61640" windowHeight="27180" activeTab="16" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="1069">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="1070">
   <si>
     <t>Screening</t>
   </si>
@@ -4916,6 +4916,9 @@
   </si>
   <si>
     <t>Secondary Objective</t>
+  </si>
+  <si>
+    <t>Exploratory Objective</t>
   </si>
 </sst>
 </file>
@@ -8645,7 +8648,7 @@
         <v>842</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>849</v>

</xml_diff>

<commit_message>
2nd part of DDF-RA-523, Quantity and Range
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_3.xlsx
+++ b/tests/integration_test_files/full_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F57A9EF-DEA1-8745-80FE-89BDEE938D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE308FE3-E66B-584B-82CA-E749F9FA5051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51380" yWindow="500" windowWidth="51200" windowHeight="27180" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="27180" firstSheet="8" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -2490,130 +2490,6 @@
   </si>
   <si>
     <t>NCI_2</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;
-  &lt;p&gt;&lt;b&gt;Title of Study:&lt;/b&gt;&lt;/p&gt;
-  &lt;p&gt;A Phase 3 Study of Nasal Glucagon (LY900018) Compared to Intramuscular Glucagon for Treatment of Insulin-induced
-    Hypoglycemia in Japanese Patients with Diabetes Mellitus&lt;/p&gt;
-  &lt;p&gt;&lt;b&gt;Rationale:&lt;/b&gt;&lt;/p&gt;
-  &lt;usdm:macro id="element" name="study_rationale" /&gt;
-  &lt;p&gt;&lt;b&gt;Objectives Endpoints:&lt;/b&gt;&lt;/p&gt;
-  &lt;table class="table"&gt;
-    &lt;tr&gt;
-      &lt;th&gt;Objectives&lt;/th&gt;
-      &lt;th&gt;Endpoints&lt;/th&gt;
-    &lt;/tr&gt;
-    &lt;tr&gt;
-      &lt;td&gt;
-        &lt;p&gt;&lt;b&gt;Primary&lt;/b&gt;&lt;/p&gt;
-        &lt;p&gt;
-          &lt;usdm:macro id="xref" name="OBJ1" klass="Objective" attribute="text"&gt;&lt;/usdm:macro&gt;
-        &lt;/p&gt;
-      &lt;/td&gt;
-      &lt;td&gt;
-        &lt;p&gt;&amp;nbsp;&lt;/p&gt;
-        &lt;p&gt;
-          &lt;usdm:macro id="xref" name="END1" klass="Endpoint" attribute="text"&gt;&lt;/usdm:macro&gt;
-        &lt;/p&gt;
-      &lt;/td&gt;
-    &lt;/tr&gt;
-    &lt;tr&gt;
-      &lt;td&gt;
-        &lt;p&gt;&lt;b&gt;Secondary&lt;/b&gt;&lt;/p&gt;
-        &lt;ul&gt;
-          &lt;li&gt;
-            &lt;p&gt;
-              &lt;usdm:macro id="xref" name="OBJ2" klass="Objective" attribute="text"&gt;&lt;/usdm:macro&gt;
-            &lt;/p&gt;
-          &lt;/li&gt;
-          &lt;li&gt;
-            &lt;p&gt;
-              &lt;usdm:macro id="xref" name="OBJ3" klass="Objective" attribute="text"&gt;&lt;/usdm:macro&gt;
-            &lt;/p&gt;
-          &lt;/li&gt;
-          &lt;li&gt;
-            &lt;p&gt;
-              &lt;usdm:macro id="xref" name="OBJ4" klass="Objective" attribute="text"&gt;&lt;/usdm:macro&gt;
-            &lt;/p&gt;
-          &lt;/li&gt;
-        &lt;/ul&gt;
-      &lt;/td&gt;
-      &lt;td&gt;
-        &lt;p&gt;&amp;nbsp;&lt;/p&gt;
-        &lt;ul&gt;
-          &lt;li&gt;
-            &lt;p&gt;
-              &lt;usdm:macro id="xref" name="END2" klass="Endpoint" attribute="text"&gt;&lt;/usdm:macro&gt;
-            &lt;/p&gt;
-          &lt;/li&gt;
-          &lt;li&gt;
-            &lt;p&gt;
-              &lt;usdm:macro id="xref" name="END3" klass="Endpoint" attribute="text"&gt;&lt;/usdm:macro&gt;
-            &lt;/p&gt;
-          &lt;/li&gt;
-          &lt;li&gt;
-            &lt;p&gt;
-              &lt;usdm:macro id="xref" name="END4" klass="Endpoint" attribute="text"&gt;&lt;/usdm:macro&gt;
-            &lt;/p&gt;
-          &lt;/li&gt;
-        &lt;/ul&gt;
-      &lt;/td&gt;
-    &lt;/tr&gt;
-  &lt;/table&gt;
-  &lt;p&gt;&lt;small&gt;Abbreviations: AE = adverse event; AUC = area under the concentration versus time curve; BG max = maximal
-      plasma glucose concentration; C max = maximal concentration; IMG = intramuscular glucagon; PD = pharmacodynamics;
-      PG = plasma glucose; PK = pharmacokinetics; SAE = serious adverse event; TEAE = treatment-emergent adverse event;
-      T max = time to maximal concentration.&lt;/small&gt;&lt;/p&gt;
-  &lt;p&gt;&lt;b&gt;Summary of Study Design:&lt;/b&gt;&lt;/p&gt;
-  &lt;p&gt;Study I8R-JE-IGBJ is a Phase 3, multicenter, randomized, open-label, active comparator, single-dose, 2-treatment,
-    2-period crossover study in Japanese patients with T1DM and patients with T2DM.&lt;/p&gt;
-  &lt;p&gt;&lt;b&gt;Treatment Arms and Planned Duration for an Individual Patient:&lt;/b&gt;&lt;/p&gt;
-  &lt;p&gt;LY900018: Single 3-mg dose; nasal administration by study site personnel&lt;br /&gt;
-    IMG (GlucaGen, Novo Nordisk A/S): Single 1-mg dose; IM injection by study site personnel&lt;/p&gt;
-  &lt;p&gt;Patients will undergo a screening examination within 28 days prior to enrollment. Patients will be administered a
-    single dose in Periods 1 and 2, which will be separated by a washout period of 3 to 14 days. Patients will return
-    for a follow-up visit 26 to 30 days after the last study treatment.&lt;/p&gt;
-  &lt;p&gt;&lt;b&gt;Number of Patients:&lt;/b&gt;&lt;/p&gt;
-  &lt;p&gt;Seventy five (&lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="STUDY_POP"
-      attribute="@plannedEnrollmentNumber/Range/maxValue"&gt;&lt;/usdm:macro&gt;) patients may be enrolled in order to have at
-    least &lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="STUDY_POP"
-      attribute="@plannedCompletionNumber/Range/maxValue"&gt;&lt;/usdm:macro&gt; patients (at least &lt;usdm:macro id="xref" klass="StudyCohort"
-      name="T1DM" attribute="@plannedCompletionNumber/Range/maxValue"&gt;&lt;/usdm:macro&gt; patients with T1DM and &lt;usdm:macro
-      id="xref" klass="StudyCohort" name="T2DM" attribute="@plannedCompletionNumber/Range/maxValue"&gt;&lt;/usdm:macro&gt;
-    T2DM, respectively) complete both periods with evaluable primary outcome. If patients discontinue from the study
-    before completion of both periods with evaluable primary outcome for any reason, the patient may be replaced.
-    Replacement
-    should not occur beyond &lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="STUDY_POP"
-      attribute="@plannedEnrollmentNumber/Range/maxValue"&gt;&lt;/usdm:macro&gt; patients enrolled, if it is expected to have at
-    least &lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="STUDY_POP"
-      attribute="@plannedCompletionNumber/Range/maxValue"&gt;&lt;/usdm:macro&gt; patients complete the study.&lt;/p&gt;
-  &lt;p&gt;&lt;b&gt;Statistical Analysis:&lt;/b&gt;&lt;/p&gt;
-  &lt;p&gt;A total of 66 completers are required in the study in order to achieve the primary objective with at least 90%
-    power using the following assumptions:&lt;/p&gt;
-  &lt;ul&gt;
-    &lt;li&gt;
-      &lt;p&gt;A treatment success rate of 98% for both treatments&lt;/p&gt;
-    &lt;/li&gt;
-    &lt;li&gt;
-      &lt;p&gt;A non-inferiority margin (NIM) of 10%&lt;/p&gt;
-    &lt;/li&gt;
-    &lt;li&gt;
-      &lt;p&gt;One-sided alpha level of 0.025&lt;/p&gt;
-    &lt;/li&gt;
-    &lt;li&gt;
-      &lt;p&gt;A within-patient correlation of zero between 2 treatment visits&lt;/p&gt;
-    &lt;/li&gt;
-  &lt;/ul&gt;
-  &lt;p&gt;The primary analysis will be a treatment comparison
-    of the percentage of patients, including both T1DM and T2DM, who achieve treatment success. The percentage of
-    patients who achieve treatment success within each treatment group and the difference in the percentages between the
-    2
-    treatment groups will be computed. A 2-sided 95% confidence interval (CI) will be obtained from the 1-sample mean of
-    the paired differences in primary outcome (1=outcome observed; 0=outcome not observed) across 2 treatment visits.
-    Non-inferiority of LY900018 will be declared if the upper limit of the 2-sided 95% CI constructed on the difference
-    in percentage (IMG - LY900018) is less than the NIM of 10%.&lt;/p&gt;
-&lt;/div&gt;"</t>
   </si>
   <si>
     <t>NCI_3</t>
@@ -2815,25 +2691,6 @@
   </si>
   <si>
     <t>NCI_11</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Seventy five (&lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="STUDY_POP"
-  attribute="@plannedEnrollmentNumber/Range/maxValue"&gt;&lt;/usdm:macro&gt;) patients may be enrolled in order to have at
-least &lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="STUDY_POP"
-  attribute="@plannedCompletionNumber/Range/maxValue"&gt;&lt;/usdm:macro&gt; patients (at least &lt;usdm:macro id="xref" klass="StudyCohort"
-  name="T1DM" attribute="@plannedCompletionNumber/Range/maxValue"&gt;&lt;/usdm:macro&gt; patients with T1DM and &lt;usdm:macro id="xref"
-  klass="StudyCohort" name="T2DM" attribute="@plannedCompletionNumber/Range/maxValue"&gt;&lt;/usdm:macro&gt;
-T2DM, respectively) complete the study. For purposes of this study, a
-completer is defined as a patient who completes both periods with evaluable primary outcome.
-If patients discontinue from the study before completion of both periods with evaluable primary
-outcome for any reason, the patient may be replaced to ensure &lt;usdm:macro id="xref" klass="StudyDesignPopulation"
-  name="STUDY_POP" attribute="@plannedCompletionNumber/Range/maxValue"&gt;&lt;/usdm:macro&gt; patients complete the study.
-The replacement patients will be assigned the same treatment sequence as the patients to be
-replaced and will complete that treatment sequence in its entirety. Replacement should not occur
-beyond &lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="STUDY_POP"
-  attribute="@plannedEnrollmentNumber/Range/maxValue"&gt;&lt;/usdm:macro&gt; patients enrolled, if it is expected to have at
-least &lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="STUDY_POP"
-  attribute="@plannedCompletionNumber/Range/maxValue"&gt;&lt;/usdm:macro&gt; patients complete the study.&lt;/p&gt;</t>
   </si>
   <si>
     <t>NCI_12</t>
@@ -5601,6 +5458,149 @@
   </si>
   <si>
     <t>spare</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;
+  &lt;p&gt;&lt;b&gt;Title of Study:&lt;/b&gt;&lt;/p&gt;
+  &lt;p&gt;A Phase 3 Study of Nasal Glucagon (LY900018) Compared to Intramuscular Glucagon for Treatment of Insulin-induced
+    Hypoglycemia in Japanese Patients with Diabetes Mellitus&lt;/p&gt;
+  &lt;p&gt;&lt;b&gt;Rationale:&lt;/b&gt;&lt;/p&gt;
+  &lt;usdm:macro id="element" name="study_rationale" /&gt;
+  &lt;p&gt;&lt;b&gt;Objectives Endpoints:&lt;/b&gt;&lt;/p&gt;
+  &lt;table class="table"&gt;
+    &lt;tr&gt;
+      &lt;th&gt;Objectives&lt;/th&gt;
+      &lt;th&gt;Endpoints&lt;/th&gt;
+    &lt;/tr&gt;
+    &lt;tr&gt;
+      &lt;td&gt;
+        &lt;p&gt;&lt;b&gt;Primary&lt;/b&gt;&lt;/p&gt;
+        &lt;p&gt;
+          &lt;usdm:macro id="xref" name="OBJ1" klass="Objective" attribute="text"&gt;&lt;/usdm:macro&gt;
+        &lt;/p&gt;
+      &lt;/td&gt;
+      &lt;td&gt;
+        &lt;p&gt;&amp;nbsp;&lt;/p&gt;
+        &lt;p&gt;
+          &lt;usdm:macro id="xref" name="END1" klass="Endpoint" attribute="text"&gt;&lt;/usdm:macro&gt;
+        &lt;/p&gt;
+      &lt;/td&gt;
+    &lt;/tr&gt;
+    &lt;tr&gt;
+      &lt;td&gt;
+        &lt;p&gt;&lt;b&gt;Secondary&lt;/b&gt;&lt;/p&gt;
+        &lt;ul&gt;
+          &lt;li&gt;
+            &lt;p&gt;
+              &lt;usdm:macro id="xref" name="OBJ2" klass="Objective" attribute="text"&gt;&lt;/usdm:macro&gt;
+            &lt;/p&gt;
+          &lt;/li&gt;
+          &lt;li&gt;
+            &lt;p&gt;
+              &lt;usdm:macro id="xref" name="OBJ3" klass="Objective" attribute="text"&gt;&lt;/usdm:macro&gt;
+            &lt;/p&gt;
+          &lt;/li&gt;
+          &lt;li&gt;
+            &lt;p&gt;
+              &lt;usdm:macro id="xref" name="OBJ4" klass="Objective" attribute="text"&gt;&lt;/usdm:macro&gt;
+            &lt;/p&gt;
+          &lt;/li&gt;
+        &lt;/ul&gt;
+      &lt;/td&gt;
+      &lt;td&gt;
+        &lt;p&gt;&amp;nbsp;&lt;/p&gt;
+        &lt;ul&gt;
+          &lt;li&gt;
+            &lt;p&gt;
+              &lt;usdm:macro id="xref" name="END2" klass="Endpoint" attribute="text"&gt;&lt;/usdm:macro&gt;
+            &lt;/p&gt;
+          &lt;/li&gt;
+          &lt;li&gt;
+            &lt;p&gt;
+              &lt;usdm:macro id="xref" name="END3" klass="Endpoint" attribute="text"&gt;&lt;/usdm:macro&gt;
+            &lt;/p&gt;
+          &lt;/li&gt;
+          &lt;li&gt;
+            &lt;p&gt;
+              &lt;usdm:macro id="xref" name="END4" klass="Endpoint" attribute="text"&gt;&lt;/usdm:macro&gt;
+            &lt;/p&gt;
+          &lt;/li&gt;
+        &lt;/ul&gt;
+      &lt;/td&gt;
+    &lt;/tr&gt;
+  &lt;/table&gt;
+  &lt;p&gt;&lt;small&gt;Abbreviations: AE = adverse event; AUC = area under the concentration versus time curve; BG max = maximal
+      plasma glucose concentration; C max = maximal concentration; IMG = intramuscular glucagon; PD = pharmacodynamics;
+      PG = plasma glucose; PK = pharmacokinetics; SAE = serious adverse event; TEAE = treatment-emergent adverse event;
+      T max = time to maximal concentration.&lt;/small&gt;&lt;/p&gt;
+  &lt;p&gt;&lt;b&gt;Summary of Study Design:&lt;/b&gt;&lt;/p&gt;
+  &lt;p&gt;Study I8R-JE-IGBJ is a Phase 3, multicenter, randomized, open-label, active comparator, single-dose, 2-treatment,
+    2-period crossover study in Japanese patients with T1DM and patients with T2DM.&lt;/p&gt;
+  &lt;p&gt;&lt;b&gt;Treatment Arms and Planned Duration for an Individual Patient:&lt;/b&gt;&lt;/p&gt;
+  &lt;p&gt;LY900018: Single 3-mg dose; nasal administration by study site personnel&lt;br /&gt;
+    IMG (GlucaGen, Novo Nordisk A/S): Single 1-mg dose; IM injection by study site personnel&lt;/p&gt;
+  &lt;p&gt;Patients will undergo a screening examination within 28 days prior to enrollment. Patients will be administered a
+    single dose in Periods 1 and 2, which will be separated by a washout period of 3 to 14 days. Patients will return
+    for a follow-up visit 26 to 30 days after the last study treatment.&lt;/p&gt;
+  &lt;p&gt;&lt;b&gt;Number of Patients:&lt;/b&gt;&lt;/p&gt;
+  &lt;p&gt;Seventy five (&lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="STUDY_POP"
+      attribute="@plannedEnrollmentNumberQuantity/Quantity/value"&gt;&lt;/usdm:macro&gt;) patients may be enrolled in order to have at
+    least &lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="STUDY_POP"
+      attribute="@plannedCompletionNumberQuantity/Quantity/value"&gt;&lt;/usdm:macro&gt; patients (at least &lt;usdm:macro id="xref" klass="StudyCohort"
+      name="T1DM" attribute="@plannedCompletionNumberQuantity/Quantity/value"&gt;&lt;/usdm:macro&gt; patients with T1DM and &lt;usdm:macro
+      id="xref" klass="StudyCohort" name="T2DM" attribute="@plannedCompletionNumberQuantity/Quantity/value"&gt;&lt;/usdm:macro&gt;
+    T2DM, respectively) complete both periods with evaluable primary outcome. If patients discontinue from the study
+    before completion of both periods with evaluable primary outcome for any reason, the patient may be replaced.
+    Replacement
+    should not occur beyond &lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="STUDY_POP"
+      attribute="@plannedEnrollmentNumberQuantity/Quantity/value"&gt;&lt;/usdm:macro&gt; patients enrolled, if it is expected to have at
+    least &lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="STUDY_POP"
+      attribute="@plannedCompletionNumberQuantity/Quantity/value"&gt;&lt;/usdm:macro&gt; patients complete the study.&lt;/p&gt;
+  &lt;p&gt;&lt;b&gt;Statistical Analysis:&lt;/b&gt;&lt;/p&gt;
+  &lt;p&gt;A total of 66 completers are required in the study in order to achieve the primary objective with at least 90%
+    power using the following assumptions:&lt;/p&gt;
+  &lt;ul&gt;
+    &lt;li&gt;
+      &lt;p&gt;A treatment success rate of 98% for both treatments&lt;/p&gt;
+    &lt;/li&gt;
+    &lt;li&gt;
+      &lt;p&gt;A non-inferiority margin (NIM) of 10%&lt;/p&gt;
+    &lt;/li&gt;
+    &lt;li&gt;
+      &lt;p&gt;One-sided alpha level of 0.025&lt;/p&gt;
+    &lt;/li&gt;
+    &lt;li&gt;
+      &lt;p&gt;A within-patient correlation of zero between 2 treatment visits&lt;/p&gt;
+    &lt;/li&gt;
+  &lt;/ul&gt;
+  &lt;p&gt;The primary analysis will be a treatment comparison
+    of the percentage of patients, including both T1DM and T2DM, who achieve treatment success. The percentage of
+    patients who achieve treatment success within each treatment group and the difference in the percentages between the
+    2
+    treatment groups will be computed. A 2-sided 95% confidence interval (CI) will be obtained from the 1-sample mean of
+    the paired differences in primary outcome (1=outcome observed; 0=outcome not observed) across 2 treatment visits.
+    Non-inferiority of LY900018 will be declared if the upper limit of the 2-sided 95% CI constructed on the difference
+    in percentage (IMG - LY900018) is less than the NIM of 10%.&lt;/p&gt;
+&lt;/div&gt;"</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Seventy five (&lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="STUDY_POP"
+  attribute="@plannedEnrollmentNumberQuantity/Quantity/value"&gt;&lt;/usdm:macro&gt;) patients may be enrolled in order to have at
+least &lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="STUDY_POP"
+  attribute="@plannedEnrollmentNumberQuantity/Quantity/value"&gt;&lt;/usdm:macro&gt; patients (at least &lt;usdm:macro id="xref" klass="StudyCohort"
+  name="T1DM" attribute="@plannedCompletionNumberQuantity/Quantity/value"&gt;&lt;/usdm:macro&gt; patients with T1DM and &lt;usdm:macro id="xref"
+  klass="StudyCohort" name="T2DM" attribute="@plannedCompletionNumberQuantity/Quantity/value"&gt;&lt;/usdm:macro&gt;
+T2DM, respectively) complete the study. For purposes of this study, a
+completer is defined as a patient who completes both periods with evaluable primary outcome.
+If patients discontinue from the study before completion of both periods with evaluable primary
+outcome for any reason, the patient may be replaced to ensure &lt;usdm:macro id="xref" klass="StudyDesignPopulation"
+  name="STUDY_POP" attribute="@plannedEnrollmentNumberQuantity/Quantity/value"&gt;&lt;/usdm:macro&gt; patients complete the study.
+The replacement patients will be assigned the same treatment sequence as the patients to be
+replaced and will complete that treatment sequence in its entirety. Replacement should not occur
+beyond &lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="STUDY_POP"
+  attribute="@plannedEnrollmentNumberQuantity/Quantity/value"&gt;&lt;/usdm:macro&gt; patients enrolled, if it is expected to have at
+least &lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="STUDY_POP"
+  attribute="@plannedEnrollmentNumberQuantity/Quantity/value"&gt;&lt;/usdm:macro&gt; patients complete the study.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -9281,7 +9281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -9803,7 +9803,7 @@
         <v>701</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>702</v>
@@ -9821,7 +9821,7 @@
         <v>705</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
     </row>
   </sheetData>
@@ -10639,8 +10639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10672,850 +10672,850 @@
         <v>765</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>766</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>766</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>767</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>769</v>
+      </c>
+      <c r="B6" s="26" t="s">
         <v>770</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>771</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="272" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>771</v>
+      </c>
+      <c r="B7" s="26" t="s">
         <v>772</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>773</v>
+      </c>
+      <c r="B8" s="26" t="s">
         <v>774</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>775</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>775</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>776</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="388" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>778</v>
+      </c>
+      <c r="B11" s="26" t="s">
         <v>779</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="289" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>782</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="255" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="170" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="187" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="238" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="221" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="221" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="B73" s="26" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="136" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="B74" s="26" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="B75" s="25" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="B76" s="25" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="B78" s="26" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B81" s="25" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="B82" s="25" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="136" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="B86" s="26"/>
     </row>
     <row r="87" spans="1:2" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="B88" s="26"/>
     </row>
     <row r="89" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="B89" s="26" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="119" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="B92" s="25" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="B93" s="25" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="119" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="B95" s="26" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="B96" s="26" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="B98" s="26" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="136" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="B99" s="26" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="B100" s="25" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="B101" s="26" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="B102" s="25" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="B103" s="26" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>948</v>
+      </c>
+      <c r="B104" s="44" t="s">
+        <v>949</v>
+      </c>
+      <c r="D104" t="s">
         <v>950</v>
-      </c>
-      <c r="B104" s="44" t="s">
-        <v>951</v>
-      </c>
-      <c r="D104" t="s">
-        <v>952</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="B105" s="26" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="B106" s="26" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="B107" s="26" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="B108" s="26" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="B109" s="26" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="B110" s="26" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="136" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="B111" s="26" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="136" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="B112" s="26" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="221" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="B113" s="26" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
   </sheetData>
@@ -11548,24 +11548,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>969</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>970</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>971</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>972</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>973</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>974</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="B2" s="27">
         <v>0</v>
@@ -11574,7 +11574,7 @@
         <v>627</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="E2" t="s">
         <v>627</v>
@@ -11585,7 +11585,7 @@
     </row>
     <row r="3" spans="1:6" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="B3" s="27">
         <v>1</v>
@@ -11594,7 +11594,7 @@
         <v>42</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="E3" t="s">
         <v>42</v>
@@ -11605,7 +11605,7 @@
     </row>
     <row r="4" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="B4" s="27">
         <v>2</v>
@@ -11614,18 +11614,18 @@
         <v>42</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="E4" t="s">
         <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B5" s="27">
         <v>3</v>
@@ -11634,78 +11634,78 @@
         <v>42</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="E5" t="s">
         <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>982</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>983</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="25" t="s">
         <v>984</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>985</v>
-      </c>
-      <c r="C6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>986</v>
-      </c>
       <c r="E6" t="s">
         <v>42</v>
       </c>
       <c r="F6" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="272" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>985</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>986</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="25" t="s">
         <v>987</v>
       </c>
-      <c r="B7" s="28" t="s">
-        <v>988</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>989</v>
-      </c>
       <c r="E7" t="s">
         <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>988</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>989</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="25" t="s">
         <v>990</v>
       </c>
-      <c r="B8" s="28" t="s">
-        <v>991</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>992</v>
-      </c>
       <c r="E8" t="s">
         <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B9" s="27">
         <v>4</v>
@@ -11714,18 +11714,18 @@
         <v>42</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="E9" t="s">
         <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="B10" s="27">
         <v>5</v>
@@ -11734,118 +11734,118 @@
         <v>42</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="E10" t="s">
         <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="388" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>995</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>996</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="25" t="s">
         <v>997</v>
       </c>
-      <c r="B11" s="28" t="s">
-        <v>998</v>
-      </c>
-      <c r="C11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>999</v>
-      </c>
       <c r="E11" t="s">
         <v>42</v>
       </c>
       <c r="F11" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="289" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>998</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>999</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="25" t="s">
         <v>1000</v>
       </c>
-      <c r="B12" s="28" t="s">
-        <v>1001</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>1002</v>
-      </c>
       <c r="E12" t="s">
         <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="25" t="s">
         <v>1003</v>
       </c>
-      <c r="B13" s="28" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>1005</v>
-      </c>
       <c r="E13" t="s">
         <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>1006</v>
       </c>
-      <c r="B14" s="28" t="s">
-        <v>1007</v>
-      </c>
-      <c r="C14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>1008</v>
-      </c>
       <c r="E14" t="s">
         <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="25" t="s">
         <v>1009</v>
       </c>
-      <c r="B15" s="28" t="s">
-        <v>1010</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>1011</v>
-      </c>
       <c r="E15" t="s">
         <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="B16" s="27">
         <v>6</v>
@@ -11854,121 +11854,121 @@
         <v>42</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="E16" t="s">
         <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="25" t="s">
         <v>1014</v>
       </c>
-      <c r="B17" s="28" t="s">
-        <v>1015</v>
-      </c>
-      <c r="C17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>1016</v>
-      </c>
       <c r="E17" t="s">
         <v>42</v>
       </c>
       <c r="F17" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>1017</v>
       </c>
-      <c r="B18" s="28" t="s">
-        <v>1018</v>
-      </c>
-      <c r="C18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>1019</v>
-      </c>
       <c r="E18" t="s">
         <v>42</v>
       </c>
       <c r="F18" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="25" t="s">
         <v>1020</v>
       </c>
-      <c r="B19" s="28" t="s">
-        <v>1021</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>1022</v>
-      </c>
       <c r="E19" t="s">
         <v>42</v>
       </c>
       <c r="F19" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="25" t="s">
         <v>1023</v>
       </c>
-      <c r="B20" s="28" t="s">
-        <v>1024</v>
-      </c>
-      <c r="C20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>1025</v>
-      </c>
       <c r="E20" t="s">
         <v>42</v>
       </c>
       <c r="F20" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="25" t="s">
         <v>1026</v>
       </c>
-      <c r="B21" s="28" t="s">
-        <v>1027</v>
-      </c>
-      <c r="C21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>1028</v>
-      </c>
       <c r="E21" t="s">
         <v>42</v>
       </c>
       <c r="F21" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="C22" t="s">
         <v>42</v>
@@ -11980,52 +11980,52 @@
         <v>42</v>
       </c>
       <c r="F22" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="25" t="s">
         <v>1031</v>
       </c>
-      <c r="B23" s="28" t="s">
-        <v>1032</v>
-      </c>
-      <c r="C23" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>1033</v>
-      </c>
       <c r="E23" t="s">
         <v>42</v>
       </c>
       <c r="F23" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="25" t="s">
         <v>1034</v>
       </c>
-      <c r="B24" s="28" t="s">
-        <v>1035</v>
-      </c>
-      <c r="C24" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>1036</v>
-      </c>
       <c r="E24" t="s">
         <v>42</v>
       </c>
       <c r="F24" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="B25" s="27">
         <v>7</v>
@@ -12034,238 +12034,238 @@
         <v>42</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="E25" t="s">
         <v>42</v>
       </c>
       <c r="F25" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="25" t="s">
         <v>1039</v>
       </c>
-      <c r="B26" s="28" t="s">
-        <v>1040</v>
-      </c>
-      <c r="C26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>1041</v>
-      </c>
       <c r="E26" t="s">
         <v>42</v>
       </c>
       <c r="F26" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="25" t="s">
         <v>1042</v>
       </c>
-      <c r="B27" s="28" t="s">
-        <v>1043</v>
-      </c>
-      <c r="C27" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>1044</v>
-      </c>
       <c r="E27" t="s">
         <v>42</v>
       </c>
       <c r="F27" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="25" t="s">
         <v>1045</v>
       </c>
-      <c r="B28" s="28" t="s">
-        <v>1046</v>
-      </c>
-      <c r="C28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>1047</v>
-      </c>
       <c r="E28" t="s">
         <v>42</v>
       </c>
       <c r="F28" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="25" t="s">
         <v>1048</v>
       </c>
-      <c r="B29" s="28" t="s">
-        <v>1049</v>
-      </c>
-      <c r="C29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>1050</v>
-      </c>
       <c r="E29" t="s">
         <v>42</v>
       </c>
       <c r="F29" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="25" t="s">
         <v>1051</v>
       </c>
-      <c r="B30" s="28" t="s">
-        <v>1052</v>
-      </c>
-      <c r="C30" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>1053</v>
-      </c>
       <c r="E30" t="s">
         <v>42</v>
       </c>
       <c r="F30" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="25" t="s">
         <v>1054</v>
       </c>
-      <c r="B31" s="28" t="s">
-        <v>1055</v>
-      </c>
-      <c r="C31" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>1056</v>
-      </c>
       <c r="E31" t="s">
         <v>42</v>
       </c>
       <c r="F31" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="25" t="s">
         <v>1057</v>
       </c>
-      <c r="B32" s="28" t="s">
-        <v>1058</v>
-      </c>
-      <c r="C32" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>1059</v>
-      </c>
       <c r="E32" t="s">
         <v>42</v>
       </c>
       <c r="F32" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="25" t="s">
         <v>1060</v>
       </c>
-      <c r="B33" s="28" t="s">
-        <v>1061</v>
-      </c>
-      <c r="C33" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>1062</v>
-      </c>
       <c r="E33" t="s">
         <v>42</v>
       </c>
       <c r="F33" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="25" t="s">
         <v>1063</v>
       </c>
-      <c r="B34" s="28" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C34" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>1065</v>
-      </c>
       <c r="E34" t="s">
         <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="255" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="25" t="s">
         <v>1066</v>
       </c>
-      <c r="B35" s="28" t="s">
-        <v>1067</v>
-      </c>
-      <c r="C35" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>1068</v>
-      </c>
       <c r="E35" t="s">
         <v>42</v>
       </c>
       <c r="F35" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="25" t="s">
         <v>1069</v>
       </c>
-      <c r="B36" s="28" t="s">
-        <v>1070</v>
-      </c>
-      <c r="C36" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" s="25" t="s">
-        <v>1071</v>
-      </c>
       <c r="E36" t="s">
         <v>42</v>
       </c>
       <c r="F36" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="B37" s="27">
         <v>8</v>
@@ -12274,118 +12274,118 @@
         <v>42</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="E37" t="s">
         <v>42</v>
       </c>
       <c r="F37" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="25" t="s">
         <v>1074</v>
       </c>
-      <c r="B38" s="28" t="s">
-        <v>1075</v>
-      </c>
-      <c r="C38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" s="25" t="s">
-        <v>1076</v>
-      </c>
       <c r="E38" t="s">
         <v>42</v>
       </c>
       <c r="F38" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B39" s="28" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="25" t="s">
         <v>1077</v>
       </c>
-      <c r="B39" s="28" t="s">
-        <v>1078</v>
-      </c>
-      <c r="C39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>1079</v>
-      </c>
       <c r="E39" t="s">
         <v>42</v>
       </c>
       <c r="F39" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="25" t="s">
         <v>1080</v>
       </c>
-      <c r="B40" s="28" t="s">
-        <v>1081</v>
-      </c>
-      <c r="C40" t="s">
-        <v>42</v>
-      </c>
-      <c r="D40" s="25" t="s">
-        <v>1082</v>
-      </c>
       <c r="E40" t="s">
         <v>42</v>
       </c>
       <c r="F40" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="25" t="s">
         <v>1083</v>
       </c>
-      <c r="B41" s="28" t="s">
-        <v>1084</v>
-      </c>
-      <c r="C41" t="s">
-        <v>42</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>1085</v>
-      </c>
       <c r="E41" t="s">
         <v>42</v>
       </c>
       <c r="F41" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="25" t="s">
         <v>1086</v>
       </c>
-      <c r="B42" s="28" t="s">
-        <v>1087</v>
-      </c>
-      <c r="C42" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>1088</v>
-      </c>
       <c r="E42" t="s">
         <v>42</v>
       </c>
       <c r="F42" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="B43" s="27">
         <v>9</v>
@@ -12394,421 +12394,421 @@
         <v>42</v>
       </c>
       <c r="D43" s="25" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="E43" t="s">
         <v>42</v>
       </c>
       <c r="F43" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B44" s="28" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C44" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="25" t="s">
         <v>1091</v>
       </c>
-      <c r="B44" s="28" t="s">
-        <v>1092</v>
-      </c>
-      <c r="C44" t="s">
-        <v>42</v>
-      </c>
-      <c r="D44" s="25" t="s">
-        <v>1093</v>
-      </c>
       <c r="E44" t="s">
         <v>42</v>
       </c>
       <c r="F44" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C45" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="25" t="s">
         <v>1094</v>
       </c>
-      <c r="B45" s="28" t="s">
-        <v>1095</v>
-      </c>
-      <c r="C45" t="s">
-        <v>42</v>
-      </c>
-      <c r="D45" s="25" t="s">
-        <v>1096</v>
-      </c>
       <c r="E45" t="s">
         <v>42</v>
       </c>
       <c r="F45" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C46" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46" s="25" t="s">
         <v>1097</v>
       </c>
-      <c r="B46" s="28" t="s">
-        <v>1098</v>
-      </c>
-      <c r="C46" t="s">
-        <v>42</v>
-      </c>
-      <c r="D46" s="25" t="s">
-        <v>1099</v>
-      </c>
       <c r="E46" t="s">
         <v>42</v>
       </c>
       <c r="F46" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B47" s="28" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C47" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" s="25" t="s">
         <v>1100</v>
       </c>
-      <c r="B47" s="28" t="s">
-        <v>1101</v>
-      </c>
-      <c r="C47" t="s">
-        <v>42</v>
-      </c>
-      <c r="D47" s="25" t="s">
-        <v>1102</v>
-      </c>
       <c r="E47" t="s">
         <v>42</v>
       </c>
       <c r="F47" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" s="25" t="s">
         <v>1103</v>
       </c>
-      <c r="B48" s="28" t="s">
-        <v>1104</v>
-      </c>
-      <c r="C48" t="s">
-        <v>42</v>
-      </c>
-      <c r="D48" s="25" t="s">
-        <v>1105</v>
-      </c>
       <c r="E48" t="s">
         <v>42</v>
       </c>
       <c r="F48" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="170" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C49" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49" s="25" t="s">
         <v>1106</v>
       </c>
-      <c r="B49" s="28" t="s">
-        <v>1107</v>
-      </c>
-      <c r="C49" t="s">
-        <v>42</v>
-      </c>
-      <c r="D49" s="25" t="s">
-        <v>1108</v>
-      </c>
       <c r="E49" t="s">
         <v>42</v>
       </c>
       <c r="F49" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B50" s="28" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C50" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" s="25" t="s">
         <v>1109</v>
       </c>
-      <c r="B50" s="28" t="s">
-        <v>1110</v>
-      </c>
-      <c r="C50" t="s">
-        <v>42</v>
-      </c>
-      <c r="D50" s="25" t="s">
-        <v>1111</v>
-      </c>
       <c r="E50" t="s">
         <v>42</v>
       </c>
       <c r="F50" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B51" s="28" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" s="25" t="s">
         <v>1112</v>
       </c>
-      <c r="B51" s="28" t="s">
-        <v>1113</v>
-      </c>
-      <c r="C51" t="s">
-        <v>42</v>
-      </c>
-      <c r="D51" s="25" t="s">
-        <v>1114</v>
-      </c>
       <c r="E51" t="s">
         <v>42</v>
       </c>
       <c r="F51" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B52" s="28" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C52" t="s">
+        <v>42</v>
+      </c>
+      <c r="D52" s="25" t="s">
         <v>1115</v>
       </c>
-      <c r="B52" s="28" t="s">
-        <v>1116</v>
-      </c>
-      <c r="C52" t="s">
-        <v>42</v>
-      </c>
-      <c r="D52" s="25" t="s">
-        <v>1117</v>
-      </c>
       <c r="E52" t="s">
         <v>42</v>
       </c>
       <c r="F52" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B53" s="28" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C53" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53" s="25" t="s">
         <v>1118</v>
       </c>
-      <c r="B53" s="28" t="s">
-        <v>1119</v>
-      </c>
-      <c r="C53" t="s">
-        <v>42</v>
-      </c>
-      <c r="D53" s="25" t="s">
-        <v>1120</v>
-      </c>
       <c r="E53" t="s">
         <v>42</v>
       </c>
       <c r="F53" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B54" s="28" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C54" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="26" t="s">
         <v>1121</v>
       </c>
-      <c r="B54" s="28" t="s">
-        <v>1122</v>
-      </c>
-      <c r="C54" t="s">
-        <v>42</v>
-      </c>
-      <c r="D54" s="26" t="s">
-        <v>1123</v>
-      </c>
       <c r="E54" t="s">
         <v>42</v>
       </c>
       <c r="F54" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B55" s="28" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C55" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" s="25" t="s">
         <v>1124</v>
       </c>
-      <c r="B55" s="28" t="s">
-        <v>1125</v>
-      </c>
-      <c r="C55" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" s="25" t="s">
-        <v>1126</v>
-      </c>
       <c r="E55" t="s">
         <v>42</v>
       </c>
       <c r="F55" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="187" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B56" s="28" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C56" t="s">
+        <v>42</v>
+      </c>
+      <c r="D56" s="25" t="s">
         <v>1127</v>
       </c>
-      <c r="B56" s="28" t="s">
-        <v>1128</v>
-      </c>
-      <c r="C56" t="s">
-        <v>42</v>
-      </c>
-      <c r="D56" s="25" t="s">
-        <v>1129</v>
-      </c>
       <c r="E56" t="s">
         <v>42</v>
       </c>
       <c r="F56" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B57" s="28" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C57" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" s="25" t="s">
         <v>1130</v>
       </c>
-      <c r="B57" s="28" t="s">
-        <v>1131</v>
-      </c>
-      <c r="C57" t="s">
-        <v>42</v>
-      </c>
-      <c r="D57" s="25" t="s">
-        <v>1132</v>
-      </c>
       <c r="E57" t="s">
         <v>42</v>
       </c>
       <c r="F57" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B58" s="28" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C58" t="s">
+        <v>42</v>
+      </c>
+      <c r="D58" s="25" t="s">
         <v>1133</v>
       </c>
-      <c r="B58" s="28" t="s">
-        <v>1134</v>
-      </c>
-      <c r="C58" t="s">
-        <v>42</v>
-      </c>
-      <c r="D58" s="25" t="s">
-        <v>1135</v>
-      </c>
       <c r="E58" t="s">
         <v>42</v>
       </c>
       <c r="F58" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B59" s="28" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C59" t="s">
+        <v>42</v>
+      </c>
+      <c r="D59" s="25" t="s">
         <v>1136</v>
       </c>
-      <c r="B59" s="28" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C59" t="s">
-        <v>42</v>
-      </c>
-      <c r="D59" s="25" t="s">
-        <v>1138</v>
-      </c>
       <c r="E59" t="s">
         <v>42</v>
       </c>
       <c r="F59" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B60" s="28" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C60" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60" s="25" t="s">
         <v>1139</v>
       </c>
-      <c r="B60" s="28" t="s">
-        <v>1140</v>
-      </c>
-      <c r="C60" t="s">
-        <v>42</v>
-      </c>
-      <c r="D60" s="25" t="s">
-        <v>1141</v>
-      </c>
       <c r="E60" t="s">
         <v>42</v>
       </c>
       <c r="F60" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B61" s="28" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C61" t="s">
+        <v>42</v>
+      </c>
+      <c r="D61" s="25" t="s">
         <v>1142</v>
       </c>
-      <c r="B61" s="28" t="s">
-        <v>1143</v>
-      </c>
-      <c r="C61" t="s">
-        <v>42</v>
-      </c>
-      <c r="D61" s="25" t="s">
-        <v>1144</v>
-      </c>
       <c r="E61" t="s">
         <v>42</v>
       </c>
       <c r="F61" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B62" s="28" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C62" t="s">
+        <v>42</v>
+      </c>
+      <c r="D62" s="25" t="s">
         <v>1145</v>
       </c>
-      <c r="B62" s="28" t="s">
-        <v>1146</v>
-      </c>
-      <c r="C62" t="s">
-        <v>42</v>
-      </c>
-      <c r="D62" s="25" t="s">
-        <v>1147</v>
-      </c>
       <c r="E62" t="s">
         <v>42</v>
       </c>
       <c r="F62" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B63" s="28" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C63" t="s">
+        <v>42</v>
+      </c>
+      <c r="D63" s="25" t="s">
         <v>1148</v>
       </c>
-      <c r="B63" s="28" t="s">
-        <v>1149</v>
-      </c>
-      <c r="C63" t="s">
-        <v>42</v>
-      </c>
-      <c r="D63" s="25" t="s">
-        <v>1150</v>
-      </c>
       <c r="E63" t="s">
         <v>42</v>
       </c>
       <c r="F63" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="B64" s="28" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="C64" t="s">
         <v>42</v>
@@ -12820,252 +12820,252 @@
         <v>42</v>
       </c>
       <c r="F64" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="238" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B65" s="28" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C65" t="s">
+        <v>42</v>
+      </c>
+      <c r="D65" s="25" t="s">
         <v>1153</v>
       </c>
-      <c r="B65" s="28" t="s">
-        <v>1154</v>
-      </c>
-      <c r="C65" t="s">
-        <v>42</v>
-      </c>
-      <c r="D65" s="25" t="s">
-        <v>1155</v>
-      </c>
       <c r="E65" t="s">
         <v>42</v>
       </c>
       <c r="F65" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B66" s="28" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C66" t="s">
+        <v>42</v>
+      </c>
+      <c r="D66" s="25" t="s">
         <v>1156</v>
       </c>
-      <c r="B66" s="28" t="s">
-        <v>1157</v>
-      </c>
-      <c r="C66" t="s">
-        <v>42</v>
-      </c>
-      <c r="D66" s="25" t="s">
-        <v>1158</v>
-      </c>
       <c r="E66" t="s">
         <v>42</v>
       </c>
       <c r="F66" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="221" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B67" s="28" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C67" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" s="25" t="s">
         <v>1159</v>
       </c>
-      <c r="B67" s="28" t="s">
-        <v>1160</v>
-      </c>
-      <c r="C67" t="s">
-        <v>42</v>
-      </c>
-      <c r="D67" s="25" t="s">
-        <v>1161</v>
-      </c>
       <c r="E67" t="s">
         <v>42</v>
       </c>
       <c r="F67" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B68" s="28" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C68" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" s="25" t="s">
         <v>1162</v>
       </c>
-      <c r="B68" s="28" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C68" t="s">
-        <v>42</v>
-      </c>
-      <c r="D68" s="25" t="s">
-        <v>1164</v>
-      </c>
       <c r="E68" t="s">
         <v>42</v>
       </c>
       <c r="F68" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B69" s="28" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C69" t="s">
+        <v>42</v>
+      </c>
+      <c r="D69" s="25" t="s">
         <v>1165</v>
       </c>
-      <c r="B69" s="28" t="s">
-        <v>1166</v>
-      </c>
-      <c r="C69" t="s">
-        <v>42</v>
-      </c>
-      <c r="D69" s="25" t="s">
-        <v>1167</v>
-      </c>
       <c r="E69" t="s">
         <v>42</v>
       </c>
       <c r="F69" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B70" s="28" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C70" t="s">
+        <v>42</v>
+      </c>
+      <c r="D70" s="25" t="s">
         <v>1168</v>
       </c>
-      <c r="B70" s="28" t="s">
-        <v>1169</v>
-      </c>
-      <c r="C70" t="s">
-        <v>42</v>
-      </c>
-      <c r="D70" s="25" t="s">
-        <v>1170</v>
-      </c>
       <c r="E70" t="s">
         <v>42</v>
       </c>
       <c r="F70" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B71" s="28" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C71" t="s">
+        <v>42</v>
+      </c>
+      <c r="D71" s="25" t="s">
         <v>1171</v>
       </c>
-      <c r="B71" s="28" t="s">
-        <v>1172</v>
-      </c>
-      <c r="C71" t="s">
-        <v>42</v>
-      </c>
-      <c r="D71" s="25" t="s">
-        <v>1173</v>
-      </c>
       <c r="E71" t="s">
         <v>42</v>
       </c>
       <c r="F71" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B72" s="28" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C72" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" s="25" t="s">
         <v>1174</v>
       </c>
-      <c r="B72" s="28" t="s">
-        <v>1175</v>
-      </c>
-      <c r="C72" t="s">
-        <v>42</v>
-      </c>
-      <c r="D72" s="25" t="s">
-        <v>1176</v>
-      </c>
       <c r="E72" t="s">
         <v>42</v>
       </c>
       <c r="F72" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="221" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B73" s="28" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C73" t="s">
+        <v>42</v>
+      </c>
+      <c r="D73" s="25" t="s">
         <v>1177</v>
       </c>
-      <c r="B73" s="28" t="s">
-        <v>1178</v>
-      </c>
-      <c r="C73" t="s">
-        <v>42</v>
-      </c>
-      <c r="D73" s="25" t="s">
-        <v>1179</v>
-      </c>
       <c r="E73" t="s">
         <v>42</v>
       </c>
       <c r="F73" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="136" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B74" s="28" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C74" t="s">
+        <v>42</v>
+      </c>
+      <c r="D74" s="25" t="s">
         <v>1180</v>
       </c>
-      <c r="B74" s="28" t="s">
-        <v>1181</v>
-      </c>
-      <c r="C74" t="s">
-        <v>42</v>
-      </c>
-      <c r="D74" s="25" t="s">
-        <v>1182</v>
-      </c>
       <c r="E74" t="s">
         <v>42</v>
       </c>
       <c r="F74" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B75" s="28" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C75" t="s">
+        <v>42</v>
+      </c>
+      <c r="D75" s="25" t="s">
         <v>1183</v>
       </c>
-      <c r="B75" s="28" t="s">
-        <v>1184</v>
-      </c>
-      <c r="C75" t="s">
-        <v>42</v>
-      </c>
-      <c r="D75" s="25" t="s">
-        <v>1185</v>
-      </c>
       <c r="E75" t="s">
         <v>42</v>
       </c>
       <c r="F75" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B76" s="28" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C76" t="s">
+        <v>42</v>
+      </c>
+      <c r="D76" s="25" t="s">
         <v>1186</v>
       </c>
-      <c r="B76" s="28" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C76" t="s">
-        <v>42</v>
-      </c>
-      <c r="D76" s="25" t="s">
-        <v>1188</v>
-      </c>
       <c r="E76" t="s">
         <v>42</v>
       </c>
       <c r="F76" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="B77" s="27">
         <v>10</v>
@@ -13074,538 +13074,538 @@
         <v>42</v>
       </c>
       <c r="D77" s="25" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E77" t="s">
         <v>42</v>
       </c>
       <c r="F77" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B78" s="28" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C78" t="s">
+        <v>42</v>
+      </c>
+      <c r="D78" s="25" t="s">
         <v>1191</v>
       </c>
-      <c r="B78" s="28" t="s">
-        <v>1192</v>
-      </c>
-      <c r="C78" t="s">
-        <v>42</v>
-      </c>
-      <c r="D78" s="25" t="s">
-        <v>1193</v>
-      </c>
       <c r="E78" t="s">
         <v>42</v>
       </c>
       <c r="F78" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B79" s="28" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C79" t="s">
+        <v>42</v>
+      </c>
+      <c r="D79" s="25" t="s">
         <v>1194</v>
       </c>
-      <c r="B79" s="28" t="s">
-        <v>1195</v>
-      </c>
-      <c r="C79" t="s">
-        <v>42</v>
-      </c>
-      <c r="D79" s="25" t="s">
-        <v>1196</v>
-      </c>
       <c r="E79" t="s">
         <v>42</v>
       </c>
       <c r="F79" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B80" s="28" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C80" t="s">
+        <v>42</v>
+      </c>
+      <c r="D80" s="25" t="s">
         <v>1197</v>
       </c>
-      <c r="B80" s="28" t="s">
-        <v>1198</v>
-      </c>
-      <c r="C80" t="s">
-        <v>42</v>
-      </c>
-      <c r="D80" s="25" t="s">
-        <v>1199</v>
-      </c>
       <c r="E80" t="s">
         <v>42</v>
       </c>
       <c r="F80" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B81" s="28" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C81" t="s">
+        <v>42</v>
+      </c>
+      <c r="D81" s="25" t="s">
         <v>1200</v>
       </c>
-      <c r="B81" s="28" t="s">
-        <v>1201</v>
-      </c>
-      <c r="C81" t="s">
-        <v>42</v>
-      </c>
-      <c r="D81" s="25" t="s">
-        <v>1202</v>
-      </c>
       <c r="E81" t="s">
         <v>42</v>
       </c>
       <c r="F81" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="B82" s="28" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="C82" t="s">
         <v>42</v>
       </c>
       <c r="D82" s="25" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="E82" t="s">
         <v>42</v>
       </c>
       <c r="F82" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="136" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B83" s="28" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C83" t="s">
+        <v>42</v>
+      </c>
+      <c r="D83" s="25" t="s">
         <v>1205</v>
       </c>
-      <c r="B83" s="28" t="s">
-        <v>1206</v>
-      </c>
-      <c r="C83" t="s">
-        <v>42</v>
-      </c>
-      <c r="D83" s="25" t="s">
-        <v>1207</v>
-      </c>
       <c r="E83" t="s">
         <v>42</v>
       </c>
       <c r="F83" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B84" s="28" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C84" t="s">
+        <v>42</v>
+      </c>
+      <c r="D84" s="25" t="s">
         <v>1208</v>
       </c>
-      <c r="B84" s="28" t="s">
-        <v>1209</v>
-      </c>
-      <c r="C84" t="s">
-        <v>42</v>
-      </c>
-      <c r="D84" s="25" t="s">
-        <v>1210</v>
-      </c>
       <c r="E84" t="s">
         <v>42</v>
       </c>
       <c r="F84" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B85" s="28" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C85" t="s">
+        <v>42</v>
+      </c>
+      <c r="D85" s="25" t="s">
         <v>1211</v>
       </c>
-      <c r="B85" s="28" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C85" t="s">
-        <v>42</v>
-      </c>
-      <c r="D85" s="25" t="s">
-        <v>1213</v>
-      </c>
       <c r="E85" t="s">
         <v>42</v>
       </c>
       <c r="F85" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B86" s="28" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C86" t="s">
+        <v>42</v>
+      </c>
+      <c r="D86" s="43" t="s">
         <v>1214</v>
       </c>
-      <c r="B86" s="28" t="s">
-        <v>1215</v>
-      </c>
-      <c r="C86" t="s">
-        <v>42</v>
-      </c>
-      <c r="D86" s="43" t="s">
-        <v>1216</v>
-      </c>
       <c r="E86" t="s">
         <v>42</v>
       </c>
       <c r="F86" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B87" s="28" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C87" t="s">
+        <v>42</v>
+      </c>
+      <c r="D87" s="43" t="s">
         <v>1217</v>
       </c>
-      <c r="B87" s="28" t="s">
-        <v>1218</v>
-      </c>
-      <c r="C87" t="s">
-        <v>42</v>
-      </c>
-      <c r="D87" s="43" t="s">
-        <v>1219</v>
-      </c>
       <c r="E87" t="s">
         <v>42</v>
       </c>
       <c r="F87" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B88" s="28" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C88" t="s">
+        <v>42</v>
+      </c>
+      <c r="D88" s="25" t="s">
         <v>1220</v>
       </c>
-      <c r="B88" s="28" t="s">
-        <v>1221</v>
-      </c>
-      <c r="C88" t="s">
-        <v>42</v>
-      </c>
-      <c r="D88" s="25" t="s">
-        <v>1222</v>
-      </c>
       <c r="E88" t="s">
         <v>42</v>
       </c>
       <c r="F88" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B89" s="28" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C89" t="s">
+        <v>42</v>
+      </c>
+      <c r="D89" s="25" t="s">
         <v>1223</v>
       </c>
-      <c r="B89" s="28" t="s">
-        <v>1224</v>
-      </c>
-      <c r="C89" t="s">
-        <v>42</v>
-      </c>
-      <c r="D89" s="25" t="s">
-        <v>1225</v>
-      </c>
       <c r="E89" t="s">
         <v>42</v>
       </c>
       <c r="F89" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B90" s="28" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C90" t="s">
+        <v>42</v>
+      </c>
+      <c r="D90" s="25" t="s">
         <v>1226</v>
       </c>
-      <c r="B90" s="28" t="s">
-        <v>1227</v>
-      </c>
-      <c r="C90" t="s">
-        <v>42</v>
-      </c>
-      <c r="D90" s="25" t="s">
-        <v>1228</v>
-      </c>
       <c r="E90" t="s">
         <v>42</v>
       </c>
       <c r="F90" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="119" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B91" s="28" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C91" t="s">
+        <v>42</v>
+      </c>
+      <c r="D91" s="25" t="s">
         <v>1229</v>
       </c>
-      <c r="B91" s="28" t="s">
-        <v>1230</v>
-      </c>
-      <c r="C91" t="s">
-        <v>42</v>
-      </c>
-      <c r="D91" s="25" t="s">
-        <v>1231</v>
-      </c>
       <c r="E91" t="s">
         <v>42</v>
       </c>
       <c r="F91" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B92" s="28" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C92" t="s">
+        <v>42</v>
+      </c>
+      <c r="D92" s="25" t="s">
         <v>1232</v>
       </c>
-      <c r="B92" s="28" t="s">
-        <v>1233</v>
-      </c>
-      <c r="C92" t="s">
-        <v>42</v>
-      </c>
-      <c r="D92" s="25" t="s">
-        <v>1234</v>
-      </c>
       <c r="E92" t="s">
         <v>42</v>
       </c>
       <c r="F92" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B93" s="28" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C93" t="s">
+        <v>42</v>
+      </c>
+      <c r="D93" s="25" t="s">
         <v>1235</v>
       </c>
-      <c r="B93" s="28" t="s">
-        <v>1236</v>
-      </c>
-      <c r="C93" t="s">
-        <v>42</v>
-      </c>
-      <c r="D93" s="25" t="s">
-        <v>1237</v>
-      </c>
       <c r="E93" t="s">
         <v>42</v>
       </c>
       <c r="F93" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B94" s="28" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C94" t="s">
+        <v>42</v>
+      </c>
+      <c r="D94" s="25" t="s">
         <v>1238</v>
       </c>
-      <c r="B94" s="28" t="s">
-        <v>1239</v>
-      </c>
-      <c r="C94" t="s">
-        <v>42</v>
-      </c>
-      <c r="D94" s="25" t="s">
-        <v>1240</v>
-      </c>
       <c r="E94" t="s">
         <v>42</v>
       </c>
       <c r="F94" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="119" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B95" s="28" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C95" t="s">
+        <v>42</v>
+      </c>
+      <c r="D95" s="25" t="s">
         <v>1241</v>
       </c>
-      <c r="B95" s="28" t="s">
-        <v>1242</v>
-      </c>
-      <c r="C95" t="s">
-        <v>42</v>
-      </c>
-      <c r="D95" s="25" t="s">
-        <v>1243</v>
-      </c>
       <c r="E95" t="s">
         <v>42</v>
       </c>
       <c r="F95" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B96" s="28" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C96" t="s">
+        <v>42</v>
+      </c>
+      <c r="D96" s="25" t="s">
         <v>1244</v>
       </c>
-      <c r="B96" s="28" t="s">
-        <v>1245</v>
-      </c>
-      <c r="C96" t="s">
-        <v>42</v>
-      </c>
-      <c r="D96" s="25" t="s">
-        <v>1246</v>
-      </c>
       <c r="E96" t="s">
         <v>42</v>
       </c>
       <c r="F96" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B97" s="28" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C97" t="s">
+        <v>42</v>
+      </c>
+      <c r="D97" s="25" t="s">
         <v>1247</v>
       </c>
-      <c r="B97" s="28" t="s">
-        <v>1248</v>
-      </c>
-      <c r="C97" t="s">
-        <v>42</v>
-      </c>
-      <c r="D97" s="25" t="s">
-        <v>1249</v>
-      </c>
       <c r="E97" t="s">
         <v>42</v>
       </c>
       <c r="F97" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B98" s="28" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C98" t="s">
+        <v>42</v>
+      </c>
+      <c r="D98" s="25" t="s">
         <v>1250</v>
       </c>
-      <c r="B98" s="28" t="s">
-        <v>1251</v>
-      </c>
-      <c r="C98" t="s">
-        <v>42</v>
-      </c>
-      <c r="D98" s="25" t="s">
-        <v>1252</v>
-      </c>
       <c r="E98" t="s">
         <v>42</v>
       </c>
       <c r="F98" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="136" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B99" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C99" t="s">
+        <v>42</v>
+      </c>
+      <c r="D99" s="25" t="s">
         <v>1253</v>
       </c>
-      <c r="B99" s="28" t="s">
-        <v>1254</v>
-      </c>
-      <c r="C99" t="s">
-        <v>42</v>
-      </c>
-      <c r="D99" s="25" t="s">
-        <v>1255</v>
-      </c>
       <c r="E99" t="s">
         <v>42</v>
       </c>
       <c r="F99" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B100" s="28" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C100" t="s">
+        <v>42</v>
+      </c>
+      <c r="D100" s="25" t="s">
         <v>1256</v>
       </c>
-      <c r="B100" s="28" t="s">
-        <v>1257</v>
-      </c>
-      <c r="C100" t="s">
-        <v>42</v>
-      </c>
-      <c r="D100" s="25" t="s">
-        <v>1258</v>
-      </c>
       <c r="E100" t="s">
         <v>42</v>
       </c>
       <c r="F100" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B101" s="28" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C101" t="s">
+        <v>42</v>
+      </c>
+      <c r="D101" s="25" t="s">
         <v>1259</v>
       </c>
-      <c r="B101" s="28" t="s">
-        <v>1260</v>
-      </c>
-      <c r="C101" t="s">
-        <v>42</v>
-      </c>
-      <c r="D101" s="25" t="s">
-        <v>1261</v>
-      </c>
       <c r="E101" t="s">
         <v>42</v>
       </c>
       <c r="F101" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B102" s="28" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C102" t="s">
+        <v>42</v>
+      </c>
+      <c r="D102" s="25" t="s">
         <v>1262</v>
       </c>
-      <c r="B102" s="28" t="s">
-        <v>1263</v>
-      </c>
-      <c r="C102" t="s">
-        <v>42</v>
-      </c>
-      <c r="D102" s="25" t="s">
-        <v>1264</v>
-      </c>
       <c r="E102" t="s">
         <v>42</v>
       </c>
       <c r="F102" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B103" s="28" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C103" t="s">
+        <v>42</v>
+      </c>
+      <c r="D103" s="25" t="s">
         <v>1265</v>
       </c>
-      <c r="B103" s="28" t="s">
-        <v>1266</v>
-      </c>
-      <c r="C103" t="s">
-        <v>42</v>
-      </c>
-      <c r="D103" s="25" t="s">
-        <v>1267</v>
-      </c>
       <c r="E103" t="s">
         <v>42</v>
       </c>
       <c r="F103" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="B104" s="27">
         <v>11</v>
@@ -13614,161 +13614,161 @@
         <v>42</v>
       </c>
       <c r="D104" s="25" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="E104" t="s">
         <v>42</v>
       </c>
       <c r="F104" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B105" s="28" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C105" t="s">
+        <v>42</v>
+      </c>
+      <c r="D105" s="25" t="s">
         <v>1270</v>
       </c>
-      <c r="B105" s="28" t="s">
-        <v>1271</v>
-      </c>
-      <c r="C105" t="s">
-        <v>42</v>
-      </c>
-      <c r="D105" s="25" t="s">
-        <v>1272</v>
-      </c>
       <c r="E105" t="s">
         <v>42</v>
       </c>
       <c r="F105" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B106" s="28" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C106" t="s">
+        <v>42</v>
+      </c>
+      <c r="D106" s="25" t="s">
         <v>1273</v>
       </c>
-      <c r="B106" s="28" t="s">
-        <v>1274</v>
-      </c>
-      <c r="C106" t="s">
-        <v>42</v>
-      </c>
-      <c r="D106" s="25" t="s">
-        <v>1275</v>
-      </c>
       <c r="E106" t="s">
         <v>42</v>
       </c>
       <c r="F106" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B107" s="28" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C107" t="s">
+        <v>42</v>
+      </c>
+      <c r="D107" s="25" t="s">
         <v>1276</v>
       </c>
-      <c r="B107" s="28" t="s">
-        <v>1277</v>
-      </c>
-      <c r="C107" t="s">
-        <v>42</v>
-      </c>
-      <c r="D107" s="25" t="s">
-        <v>1278</v>
-      </c>
       <c r="E107" t="s">
         <v>42</v>
       </c>
       <c r="F107" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B108" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C108" t="s">
+        <v>42</v>
+      </c>
+      <c r="D108" s="25" t="s">
         <v>1279</v>
       </c>
-      <c r="B108" s="28" t="s">
-        <v>1280</v>
-      </c>
-      <c r="C108" t="s">
-        <v>42</v>
-      </c>
-      <c r="D108" s="25" t="s">
-        <v>1281</v>
-      </c>
       <c r="E108" t="s">
         <v>42</v>
       </c>
       <c r="F108" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B109" s="28" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C109" t="s">
+        <v>42</v>
+      </c>
+      <c r="D109" s="25" t="s">
         <v>1282</v>
       </c>
-      <c r="B109" s="28" t="s">
-        <v>1283</v>
-      </c>
-      <c r="C109" t="s">
-        <v>42</v>
-      </c>
-      <c r="D109" s="25" t="s">
-        <v>1284</v>
-      </c>
       <c r="E109" t="s">
         <v>42</v>
       </c>
       <c r="F109" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="B110" s="28" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="C110" t="s">
         <v>42</v>
       </c>
       <c r="D110" s="25" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="E110" t="s">
         <v>42</v>
       </c>
       <c r="F110" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="136" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B111" s="28" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C111" t="s">
+        <v>42</v>
+      </c>
+      <c r="D111" s="25" t="s">
         <v>1287</v>
       </c>
-      <c r="B111" s="28" t="s">
-        <v>1288</v>
-      </c>
-      <c r="C111" t="s">
-        <v>42</v>
-      </c>
-      <c r="D111" s="25" t="s">
-        <v>1289</v>
-      </c>
       <c r="E111" t="s">
         <v>42</v>
       </c>
       <c r="F111" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="136" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B112" s="28" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="C112" t="s">
         <v>42</v>
@@ -13780,27 +13780,27 @@
         <v>42</v>
       </c>
       <c r="F112" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="221" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B113" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C113" t="s">
+        <v>42</v>
+      </c>
+      <c r="D113" s="26" t="s">
         <v>1292</v>
       </c>
-      <c r="B113" s="28" t="s">
-        <v>1293</v>
-      </c>
-      <c r="C113" t="s">
-        <v>42</v>
-      </c>
-      <c r="D113" s="26" t="s">
-        <v>1294</v>
-      </c>
       <c r="E113" t="s">
         <v>42</v>
       </c>
       <c r="F113" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
     </row>
   </sheetData>
@@ -13856,7 +13856,7 @@
         <v>53</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="E2" t="s">
         <v>54</v>
@@ -13909,7 +13909,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -13917,7 +13917,7 @@
         <v>55</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -13937,7 +13937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -14014,7 +14014,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="B7" s="45" t="s">
         <v>74</v>
@@ -14080,7 +14080,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="B13" s="45"/>
       <c r="C13" s="46"/>
@@ -14161,11 +14161,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B9:E9"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
@@ -14174,6 +14169,11 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -14184,7 +14184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>

</xml_diff>